<commit_message>
Updated the solution for Implement Atoi problem
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF788C84-2D9B-4D02-8969-3891376C8D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37CBEB9-72F3-490A-B407-66C884D1E546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
   <si>
     <t>Problem</t>
   </si>
@@ -612,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1096,9 +1096,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1111,6 +1116,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Sort 0s, 1s and 2s problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37CBEB9-72F3-490A-B407-66C884D1E546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860499C3-5C9F-4773-BA60-55F43139883A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="78">
   <si>
     <t>Problem</t>
   </si>
@@ -1096,7 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1150,9 +1150,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1165,6 +1170,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Search in Rotated Sorted Array problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860499C3-5C9F-4773-BA60-55F43139883A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F72098-AAC4-4317-88C2-C2CB47633DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
   <si>
     <t>Problem</t>
   </si>
@@ -1150,13 +1150,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5 B2:B6 B2:B7 B2:B11" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>"Done,Not Done,NA"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1169,61 +1228,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5 B2:B6 B2:B7 B2:B11" xr:uid="{00000000-0002-0000-0200-000000000000}">
-      <formula1>"Done,Not Done,NA"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Spirally traversing a matrix problem
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F72098-AAC4-4317-88C2-C2CB47633DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09AC470-938D-45DA-B9A4-5AF0F6C16D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
   <si>
     <t>Problem</t>
   </si>
@@ -1209,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1268,9 +1268,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1283,6 +1289,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Find all pairs with a given sum problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09AC470-938D-45DA-B9A4-5AF0F6C16D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91F570C-0D19-46FA-A14E-7FB550F15388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
   <si>
     <t>Problem</t>
   </si>
@@ -1268,7 +1268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1318,9 +1318,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="47.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1333,6 +1339,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Triplet Sum in Array problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91F570C-0D19-46FA-A14E-7FB550F15388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94ED32CB-E823-49CD-BA85-03C0E3C88BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="78">
   <si>
     <t>Problem</t>
   </si>
@@ -1318,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1373,9 +1373,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1388,6 +1394,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Linked List Group Reverse problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94ED32CB-E823-49CD-BA85-03C0E3C88BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239904A7-9E3E-4B23-8F6C-2788606A537C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
   <si>
     <t>Problem</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Not Done</t>
   </si>
 </sst>
 </file>
@@ -1373,7 +1376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1423,9 +1426,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1438,6 +1446,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1464,9 +1475,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="39.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1479,6 +1496,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Merge K sorted linked lists problems.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F894D7-F87F-4526-A9D1-174E987B000F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEF3ABA-DB3F-4C04-8681-D6296CB0F1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="79">
   <si>
     <t>Problem</t>
   </si>
@@ -670,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -718,6 +718,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -771,9 +775,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -786,6 +795,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Longest valid Parentheses problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEF3ABA-DB3F-4C04-8681-D6296CB0F1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE1A9F0-F6D2-4987-A1DB-FD195BD2B193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
   <si>
     <t>Problem</t>
   </si>
@@ -775,13 +775,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5 B2:B6 B2:B7 B2:B11" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+      <formula1>"Done,Not Done,NA"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -794,51 +844,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5 B2:B6 B2:B7 B2:B11" xr:uid="{00000000-0002-0000-0B00-000000000000}">
-      <formula1>"Done,Not Done,NA"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Subset Sum Problem problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE1A9F0-F6D2-4987-A1DB-FD195BD2B193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B762BD20-88EF-4B27-B79F-CE84A17CD7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
   <si>
     <t>Problem</t>
   </si>
@@ -824,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -879,9 +879,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -894,6 +899,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -915,9 +923,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="41.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -930,6 +943,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Minimum Platforms problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B762BD20-88EF-4B27-B79F-CE84A17CD7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F38D36-18DA-4C4E-A153-60A575E3DA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
   <si>
     <t>Problem</t>
   </si>
@@ -923,7 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1007,9 +1007,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1022,6 +1028,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Stock Buy and Sell - Multiple Transactions Allowed problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F38D36-18DA-4C4E-A153-60A575E3DA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1143E046-39AA-4D42-BB66-4BB2C00D93BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="79">
   <si>
     <t>Problem</t>
   </si>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,6 +645,9 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1007,7 +1010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the solution for Anagram problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1143E046-39AA-4D42-BB66-4BB2C00D93BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710F29A4-D678-4AFF-90DE-F7C45011BE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
   <si>
     <t>Problem</t>
   </si>
@@ -615,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1157,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1185,6 +1185,9 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Count Inversions problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710F29A4-D678-4AFF-90DE-F7C45011BE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42C7B66-2736-47F7-A5DF-C675106085FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
   <si>
     <t>Problem</t>
   </si>
@@ -1157,7 +1157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1242,6 +1242,9 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Peak element problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42C7B66-2736-47F7-A5DF-C675106085FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A552ACF3-5187-4544-85F1-FC70D9DD5456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="79">
   <si>
     <t>Problem</t>
   </si>
@@ -1214,7 +1214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1304,6 +1304,9 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Search in a Row-Column sorted matrix problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A552ACF3-5187-4544-85F1-FC70D9DD5456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC03AA4-9B13-46B7-93FC-29775A3855C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="79">
   <si>
     <t>Problem</t>
   </si>
@@ -1276,7 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1338,7 +1338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1368,6 +1368,9 @@
       <c r="A3" t="s">
         <v>21</v>
       </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
Updated the solution for Longest substring with distinct characters problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC03AA4-9B13-46B7-93FC-29775A3855C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF6B9E8-475F-4AEA-BD42-12E233438EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="81">
   <si>
     <t>Problem</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>Not Done</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Not relavant</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1389,27 +1395,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="47.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1417,17 +1424,23 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1446,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1476,6 +1489,9 @@
       <c r="A3" t="s">
         <v>28</v>
       </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
Updated the solution for Segregate even and odd nodes in a Linked List problem.
</commit_message>
<xml_diff>
--- a/DSA_Problems.xlsx
+++ b/DSA_Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF6B9E8-475F-4AEA-BD42-12E233438EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56C9061-2A82-4945-A347-A60855E19D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
   <si>
     <t>Problem</t>
   </si>
@@ -271,9 +271,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>Not Done</t>
   </si>
   <si>
     <t>NA</t>
@@ -1429,10 +1426,10 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
         <v>79</v>
-      </c>
-      <c r="C3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1459,7 +1456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1513,7 +1510,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1541,6 +1538,9 @@
       <c r="A3" t="s">
         <v>31</v>
       </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1561,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1591,6 +1591,9 @@
       <c r="A3" t="s">
         <v>34</v>
       </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">

</xml_diff>